<commit_message>
update to include other fields
</commit_message>
<xml_diff>
--- a/inputs/New UG Subject Codes 2025-2026.xlsx
+++ b/inputs/New UG Subject Codes 2025-2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jspenc35\projects\curriculog_excel_sheet_generator\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD3D814-603F-4681-826D-B0553C1E6993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0FDE4E-B089-4FDB-BDBD-EF33434C8384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="178">
   <si>
     <t>Field</t>
   </si>
@@ -1068,11 +1068,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B809DB27-F851-4238-909D-DC6D276C789A}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1148,29 +1148,44 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G11" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
         <v>59</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1183,43 +1198,43 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$B$4:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B75:B299</xm:sqref>
+          <xm:sqref>B76:B300</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use this to include an additional field from the proposal as a comment in the cell. Good for fields in the proposal that has lots of text.  " xr:uid="{B019C073-487B-47B8-8ABF-602FE6834B7C}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F26 F2:F6 F7:F12</xm:sqref>
+          <xm:sqref>F16:F27 F2:F13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field to separate sheets by. Creates a separate sheet for each unique value in the field. If the field is &quot;College&quot; and the proposals are from A&amp;S and Tickle Engineering, a sheet titled A&amp;S and a sheet titled Tickle Engineering are created." xr:uid="{CCE53851-1D4A-4889-8217-59A49DFAA977}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>J14 J2:J6 J7:J12</xm:sqref>
+          <xm:sqref>J15 J2:J13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select the field from the proposal you want in your Excel spreadsheet._x000a_" xr:uid="{ED19FA7F-0466-4F44-81DE-819E52E3AFC1}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A10 A13:A80</xm:sqref>
+          <xm:sqref>A14:A81 A2:A11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBF6BF9F-3BCF-40E3-BF58-E25772258781}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G6 G7:G1048576</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select how you want to filter data for in field. If you are using IN or BETWEEN use a comma-separated list. For BETWEEN put the lower end of your range first., e.g.: 2,5." xr:uid="{FEA64857-E951-453F-B873-F85426215CF0}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B6 B7:B74</xm:sqref>
+          <xm:sqref>B2:B75</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A32929B-C51D-4A5A-BFA3-4B20B2A647A4}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H6 H7:H29</xm:sqref>
+          <xm:sqref>H2:H30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>